<commit_message>
update figures; add table of taxa
</commit_message>
<xml_diff>
--- a/R/output/Table_diversity_stats.xlsx
+++ b/R/output/Table_diversity_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mawha\Dropbox\Martone Lab\martone_calvert\R\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9882C8D9-3FED-4264-9BB6-6DDB80900A74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D25B34-EC08-44D8-A9E8-FFC6A5DCD81F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{AFEBDCFD-7745-4AB4-BA4A-950277C8252B}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="10140" xr2:uid="{AFEBDCFD-7745-4AB4-BA4A-950277C8252B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,15 +48,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Year (linear)</t>
-  </si>
-  <si>
-    <t>Year (factor)</t>
-  </si>
-  <si>
     <t>Year=2013</t>
   </si>
   <si>
@@ -91,6 +82,15 @@
   </si>
   <si>
     <t>sqrt(Richness)</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>Year variable</t>
   </si>
 </sst>
 </file>
@@ -98,7 +98,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -190,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -204,13 +204,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -220,10 +220,12 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -546,19 +548,19 @@
       <selection activeCell="A2" sqref="A2:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.26953125" customWidth="1"/>
+    <col min="6" max="6" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.54296875" customWidth="1"/>
+    <col min="8" max="8" width="7.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
@@ -566,9 +568,9 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -580,24 +582,24 @@
         <v>0</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>2</v>
@@ -615,15 +617,15 @@
         <v>16.576000000000001</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>6</v>
@@ -644,9 +646,9 @@
         <v>8.7099999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
@@ -667,12 +669,12 @@
         <v>14.371</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>5</v>
@@ -692,16 +694,16 @@
       <c r="G6" s="10">
         <v>-4.069</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H6" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>2</v>
@@ -719,18 +721,18 @@
         <v>16.27</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D8" s="6">
         <v>8.2019999999999992E-3</v>
@@ -748,15 +750,15 @@
         <v>0.92290000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D9" s="6">
         <v>9.3719999999999998E-2</v>
@@ -774,15 +776,15 @@
         <v>0.26898</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="D10" s="6">
         <v>-4.5373999999999998E-2</v>
@@ -800,15 +802,15 @@
         <v>0.59240999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" s="6">
         <v>-0.22078300000000001</v>
@@ -822,19 +824,19 @@
       <c r="G11" s="6">
         <v>-2.6059999999999999</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="16">
         <v>9.3500000000000007E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D12" s="6">
         <v>-0.12618299999999999</v>
@@ -852,15 +854,15 @@
         <v>0.13680999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D13" s="6">
         <v>5.3563E-2</v>
@@ -878,15 +880,15 @@
         <v>0.52742</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D14" s="10">
         <v>-0.104708</v>
@@ -904,9 +906,9 @@
         <v>0.21687999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>5</v>
@@ -927,18 +929,18 @@
         <v>14.084</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D16" s="6">
         <v>-1.44E-2</v>
@@ -956,15 +958,15 @@
         <v>0.81616999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D17" s="6">
         <v>4.122E-2</v>
@@ -982,15 +984,15 @@
         <v>0.50582000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D18" s="6">
         <v>-0.11093</v>
@@ -1008,15 +1010,15 @@
         <v>7.3669999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D19" s="6">
         <v>-0.20263</v>
@@ -1030,19 +1032,19 @@
       <c r="G19" s="6">
         <v>-3.2719999999999998</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="16">
         <v>1.1199999999999999E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D20" s="6">
         <v>-0.14793000000000001</v>
@@ -1056,19 +1058,19 @@
       <c r="G20" s="6">
         <v>-2.3889999999999998</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="16">
         <v>1.7160000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D21" s="6">
         <v>-5.6559999999999999E-2</v>
@@ -1086,29 +1088,29 @@
         <v>0.36135</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="6">
+      <c r="C22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="10">
         <v>-0.20788999999999999</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="10">
         <v>6.1920000000000003E-2</v>
       </c>
-      <c r="F22" s="4">
-        <v>704</v>
-      </c>
-      <c r="G22" s="6">
+      <c r="F22" s="8">
+        <v>704</v>
+      </c>
+      <c r="G22" s="10">
         <v>-3.3570000000000002</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="17">
         <v>8.3000000000000001E-4</v>
       </c>
     </row>

</xml_diff>